<commit_message>
Replaced mimetype enum (which was fixed and made no sense) by string + constants to help in readability
</commit_message>
<xml_diff>
--- a/MR3/Extensions/OData/tests/test odata stuff.xlsx
+++ b/MR3/Extensions/OData/tests/test odata stuff.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="missing" sheetId="1" r:id="rId1"/>
     <sheet name="test plan" sheetId="2" r:id="rId2"/>
+    <sheet name="bugs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="111">
   <si>
     <t>Missing features</t>
   </si>
@@ -350,12 +351,24 @@
   <si>
     <t>plain</t>
   </si>
+  <si>
+    <t>Known bugs</t>
+  </si>
+  <si>
+    <t>Self referential models generate the wrong edm metadata</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Fixed?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +461,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -493,7 +514,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -543,11 +564,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -555,9 +579,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -1101,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,10 +1148,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="15"/>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="21"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="18"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
@@ -1176,16 +1198,16 @@
       <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="H5" s="24" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="H5" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="24"/>
+      <c r="I5" s="25"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
@@ -1317,10 +1339,10 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="21" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -2027,12 +2049,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C31:F31"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="C45:F45"/>
@@ -2040,8 +2056,57 @@
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="55.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
a few more tests for json serialization
</commit_message>
<xml_diff>
--- a/MR3/Extensions/OData/tests/test odata stuff.xlsx
+++ b/MR3/Extensions/OData/tests/test odata stuff.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="19200" windowHeight="9525" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="19200" windowHeight="9525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="missing" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="114">
   <si>
     <t>Missing features</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>Json serialization support</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -1129,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,6 +1254,9 @@
       <c r="B7" s="9" t="s">
         <v>101</v>
       </c>
+      <c r="C7" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="F7" s="4" t="s">
         <v>19</v>
       </c>
@@ -1271,6 +1277,9 @@
       <c r="B8" s="9" t="s">
         <v>101</v>
       </c>
+      <c r="C8" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="F8" s="4" t="s">
         <v>19</v>
       </c>
@@ -1289,6 +1298,9 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>101</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -2076,10 +2088,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E6"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2090,12 +2102,12 @@
     <col min="5" max="5" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="22" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
         <v>58</v>
       </c>
@@ -2106,12 +2118,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>111</v>
       </c>
@@ -2119,7 +2131,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
       <c r="B6" t="s">
         <v>112</v>
       </c>

</xml_diff>

<commit_message>
better content negotiation support (in progress)
</commit_message>
<xml_diff>
--- a/MR3/Extensions/OData/tests/test odata stuff.xlsx
+++ b/MR3/Extensions/OData/tests/test odata stuff.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="115">
   <si>
     <t>Missing features</t>
   </si>
@@ -364,20 +364,23 @@
     <t>Fixed?</t>
   </si>
   <si>
-    <t>Serialization of collection of complex types</t>
-  </si>
-  <si>
     <t>Json serialization support</t>
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>ATOM De/Serialization of collection of complex types</t>
+  </si>
+  <si>
+    <t>Json De/Serialization of collection of complex types</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,6 +481,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -523,7 +533,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -577,16 +587,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1132,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,10 +1171,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="15"/>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="23"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="18"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
@@ -1559,12 +1573,12 @@
     </row>
     <row r="23" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1607,12 +1621,12 @@
     </row>
     <row r="27" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1664,12 +1678,12 @@
     </row>
     <row r="31" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -1745,12 +1759,12 @@
     </row>
     <row r="37" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -1857,12 +1871,12 @@
     </row>
     <row r="45" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -1905,12 +1919,12 @@
     </row>
     <row r="49" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -1949,12 +1963,12 @@
     </row>
     <row r="53" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="24" t="s">
+      <c r="C53" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
       <c r="I53" s="13"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -1983,12 +1997,12 @@
     </row>
     <row r="57" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
-      <c r="C57" s="24" t="s">
+      <c r="C57" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -2004,12 +2018,12 @@
     </row>
     <row r="60" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="24" t="s">
+      <c r="C60" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -2048,12 +2062,12 @@
     </row>
     <row r="64" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
       <c r="I64" s="13"/>
     </row>
     <row r="65" spans="9:11" x14ac:dyDescent="0.25">
@@ -2067,12 +2081,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C31:F31"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="C45:F45"/>
@@ -2080,6 +2088,12 @@
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2088,14 +2102,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E6"/>
+  <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="28"/>
     <col min="2" max="2" width="55.28515625" customWidth="1"/>
     <col min="3" max="3" width="10" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="4" customWidth="1"/>
@@ -2125,21 +2140,26 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="28" t="s">
         <v>112</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>111</v>
       </c>
       <c r="C6" s="4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First test filtering entityset is passing.
</commit_message>
<xml_diff>
--- a/MR3/Extensions/OData/tests/test odata stuff.xlsx
+++ b/MR3/Extensions/OData/tests/test odata stuff.xlsx
@@ -587,20 +587,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1146,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,10 +1171,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="15"/>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="18"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
@@ -1221,16 +1221,16 @@
       <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="H5" s="26" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="H5" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="26"/>
+      <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
@@ -1573,12 +1573,12 @@
     </row>
     <row r="23" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1621,12 +1621,12 @@
     </row>
     <row r="27" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1678,12 +1678,12 @@
     </row>
     <row r="31" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -1759,12 +1759,12 @@
     </row>
     <row r="37" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -1871,12 +1871,12 @@
     </row>
     <row r="45" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
-      <c r="C45" s="23" t="s">
+      <c r="C45" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -1919,12 +1919,12 @@
     </row>
     <row r="49" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -1963,12 +1963,12 @@
     </row>
     <row r="53" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="23" t="s">
+      <c r="C53" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
       <c r="I53" s="13"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -1997,12 +1997,12 @@
     </row>
     <row r="57" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
-      <c r="C57" s="23" t="s">
+      <c r="C57" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="23"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -2018,12 +2018,12 @@
     </row>
     <row r="60" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="23" t="s">
+      <c r="C60" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -2062,12 +2062,12 @@
     </row>
     <row r="64" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="23" t="s">
+      <c r="C64" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
       <c r="I64" s="13"/>
     </row>
     <row r="65" spans="9:11" x14ac:dyDescent="0.25">
@@ -2081,6 +2081,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C31:F31"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="C45:F45"/>
@@ -2088,12 +2094,6 @@
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2110,7 +2110,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="28"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
     <col min="2" max="2" width="55.28515625" customWidth="1"/>
     <col min="3" max="3" width="10" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="4" customWidth="1"/>
@@ -2147,10 +2147,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="23" t="s">
         <v>111</v>
       </c>
       <c r="C6" s="4">

</xml_diff>

<commit_message>
tests for linq expressions generated. lots of fixes.
</commit_message>
<xml_diff>
--- a/MR3/Extensions/OData/tests/test odata stuff.xlsx
+++ b/MR3/Extensions/OData/tests/test odata stuff.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="19200" windowHeight="9525" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="19200" windowHeight="9525" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="missing" sheetId="1" r:id="rId1"/>
     <sheet name="test plan" sheetId="2" r:id="rId2"/>
     <sheet name="bugs" sheetId="3" r:id="rId3"/>
+    <sheet name="filtering tests" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="159">
   <si>
     <t>Missing features</t>
   </si>
@@ -375,12 +376,144 @@
   <si>
     <t>Json De/Serialization of collection of complex types</t>
   </si>
+  <si>
+    <t>Filtering tests</t>
+  </si>
+  <si>
+    <t>Negate</t>
+  </si>
+  <si>
+    <t>Unary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not </t>
+  </si>
+  <si>
+    <t>Cast</t>
+  </si>
+  <si>
+    <t>int32</t>
+  </si>
+  <si>
+    <t>int64</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>Guid</t>
+  </si>
+  <si>
+    <t>sbyte</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>DtOffset</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>gt</t>
+  </si>
+  <si>
+    <t>le</t>
+  </si>
+  <si>
+    <t>ge</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>sub</t>
+  </si>
+  <si>
+    <t>eq</t>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>Equality</t>
+  </si>
+  <si>
+    <t>Relational</t>
+  </si>
+  <si>
+    <t>Multiplicative</t>
+  </si>
+  <si>
+    <t>Additive</t>
+  </si>
+  <si>
+    <t>Conditional</t>
+  </si>
+  <si>
+    <t>mod</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>mul</t>
+  </si>
+  <si>
+    <t>both sides should be booleans</t>
+  </si>
+  <si>
+    <t>same rules, but exp is typed as bool</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,8 +621,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,6 +667,18 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -533,7 +707,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -591,17 +765,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1146,7 +1353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1171,10 +1378,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="15"/>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="26"/>
       <c r="I1" s="18"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
@@ -1573,12 +1780,12 @@
     </row>
     <row r="23" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1621,12 +1828,12 @@
     </row>
     <row r="27" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1678,12 +1885,12 @@
     </row>
     <row r="31" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -1759,12 +1966,12 @@
     </row>
     <row r="37" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -1871,12 +2078,12 @@
     </row>
     <row r="45" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -1919,12 +2126,12 @@
     </row>
     <row r="49" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -1963,12 +2170,12 @@
     </row>
     <row r="53" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
       <c r="I53" s="13"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -1997,12 +2204,12 @@
     </row>
     <row r="57" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
-      <c r="C57" s="26" t="s">
+      <c r="C57" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -2018,12 +2225,12 @@
     </row>
     <row r="60" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="26"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -2062,12 +2269,12 @@
     </row>
     <row r="64" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="26" t="s">
+      <c r="C64" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="26"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="26"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
       <c r="I64" s="13"/>
     </row>
     <row r="65" spans="9:11" x14ac:dyDescent="0.25">
@@ -2081,12 +2288,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C31:F31"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="C45:F45"/>
@@ -2094,6 +2295,12 @@
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2166,4 +2373,475 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:S28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="24" customWidth="1"/>
+    <col min="5" max="14" width="8.28515625" style="4" customWidth="1"/>
+    <col min="15" max="19" width="9.5703125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="35"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="2:19" s="41" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="M4" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="N4" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="O4" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="P4" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q4" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="R4" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="S4" s="40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="32"/>
+      <c r="C8" s="36"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="C9" s="36"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="32"/>
+      <c r="C10" s="36"/>
+      <c r="E10" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="24"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="K11" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="32"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K12" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="32"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K13" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K14" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="32"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K15" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E16" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="K16" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E17" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="K17" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="24"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="L19" s="24"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="32"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="L20" s="24"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="32"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="L21" s="24"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="32"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="L22" s="24"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="32"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="32"/>
+      <c r="C26" s="36"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="32"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to reflect tests implemented
</commit_message>
<xml_diff>
--- a/MR3/Extensions/OData/tests/test odata stuff.xlsx
+++ b/MR3/Extensions/OData/tests/test odata stuff.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="164">
   <si>
     <t>Missing features</t>
   </si>
@@ -508,12 +508,27 @@
   <si>
     <t>same rules, but exp is typed as bool</t>
   </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Promotions</t>
+  </si>
+  <si>
+    <t>S = just works</t>
+  </si>
+  <si>
+    <t>P = promotes</t>
+  </si>
+  <si>
+    <t>F = must fail</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,8 +665,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -681,8 +720,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -699,15 +743,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -765,19 +825,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -790,14 +837,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -810,13 +853,53 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="5" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1378,10 +1461,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="15"/>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="26"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="18"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
@@ -1428,16 +1511,16 @@
       <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="H5" s="28" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="H5" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="28"/>
+      <c r="I5" s="38"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
@@ -1780,12 +1863,12 @@
     </row>
     <row r="23" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1828,12 +1911,12 @@
     </row>
     <row r="27" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1885,12 +1968,12 @@
     </row>
     <row r="31" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -1966,12 +2049,12 @@
     </row>
     <row r="37" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -2078,12 +2161,12 @@
     </row>
     <row r="45" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -2126,12 +2209,12 @@
     </row>
     <row r="49" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -2170,12 +2253,12 @@
     </row>
     <row r="53" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="25" t="s">
+      <c r="C53" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
       <c r="I53" s="13"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -2204,12 +2287,12 @@
     </row>
     <row r="57" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
-      <c r="C57" s="25" t="s">
+      <c r="C57" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -2225,12 +2308,12 @@
     </row>
     <row r="60" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -2269,12 +2352,12 @@
     </row>
     <row r="64" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="25" t="s">
+      <c r="C64" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="36"/>
       <c r="I64" s="13"/>
     </row>
     <row r="65" spans="9:11" x14ac:dyDescent="0.25">
@@ -2288,6 +2371,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C31:F31"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="C45:F45"/>
@@ -2295,12 +2384,6 @@
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2312,7 +2395,7 @@
   <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,140 +2460,166 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S28"/>
+  <dimension ref="B2:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="28" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="24" customWidth="1"/>
     <col min="5" max="14" width="8.28515625" style="4" customWidth="1"/>
     <col min="15" max="19" width="9.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="2:19" s="44" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="35"/>
+      <c r="C3" s="29"/>
       <c r="E3" s="24"/>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="2:19" s="41" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40" t="s">
+    <row r="4" spans="2:19" s="34" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="J4" s="40" t="s">
+      <c r="J4" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="K4" s="40" t="s">
+      <c r="K4" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="L4" s="40" t="s">
+      <c r="L4" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="M4" s="40" t="s">
+      <c r="M4" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="N4" s="40" t="s">
+      <c r="N4" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="O4" s="40" t="s">
+      <c r="O4" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="P4" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="Q4" s="40" t="s">
+      <c r="Q4" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="R4" s="40" t="s">
+      <c r="R4" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="S4" s="40" t="s">
+      <c r="S4" s="33" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>135</v>
+      <c r="E5" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6" s="31" t="s">
-        <v>137</v>
+      <c r="E6" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="25" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="30"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="36"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="30"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="30"/>
       <c r="E10" s="24" t="s">
         <v>127</v>
       </c>
@@ -2535,50 +2644,45 @@
       <c r="L10" s="24"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="G11" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="L11" s="24" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="45" t="s">
         <v>127</v>
       </c>
+      <c r="E11" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F12" s="31" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="26" t="s">
         <v>137</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -2593,26 +2697,25 @@
       <c r="J12" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="K12" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>120</v>
+      <c r="K12" s="25" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="32"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" s="30" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>135</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="26" t="s">
         <v>137</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -2624,24 +2727,19 @@
       <c r="J13" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="K13" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>121</v>
+      <c r="K13" s="25" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="E14" s="30" t="s">
+      <c r="B14" s="27"/>
+      <c r="C14" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="25" t="s">
         <v>135</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -2650,7 +2748,7 @@
       <c r="G14" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="26" t="s">
         <v>137</v>
       </c>
       <c r="I14" s="4" t="s">
@@ -2659,20 +2757,17 @@
       <c r="J14" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="K14" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="L14" s="24" t="s">
-        <v>122</v>
+      <c r="K14" s="25" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" s="30" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="25" t="s">
         <v>135</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -2684,21 +2779,23 @@
       <c r="H15" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="26" t="s">
         <v>137</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="K15" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>123</v>
+      <c r="K15" s="25" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E16" s="30" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="25" t="s">
         <v>135</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -2713,135 +2810,342 @@
       <c r="I16" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="J16" s="31" t="s">
+      <c r="J16" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="K16" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="L16" s="24" t="s">
+      <c r="K16" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="27"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="27"/>
+      <c r="C18" s="30"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="L18" s="24"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="27"/>
+      <c r="C19" s="30"/>
+      <c r="E19" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="J19" s="24" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="L17" s="24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L18" s="24"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="32" t="s">
+      <c r="K19" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="L19" s="24"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C20" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D21" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="L21" s="24"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="27"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="27"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="27"/>
+      <c r="C24" s="30"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D26" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="27"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="E30" s="47" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="27"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="L19" s="24"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="24" t="s">
+      <c r="E31" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="27"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="L20" s="24"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="32"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="24" t="s">
+      <c r="E32" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="27"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="L21" s="24"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="32"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="24" t="s">
+      <c r="E33" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D34" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="L22" s="24"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L23" s="24"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="32" t="s">
+      <c r="E34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C36" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="E36" s="47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="27"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="E24" s="37" t="s">
+      <c r="E37" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="27"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="27"/>
+      <c r="C39" s="30"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="E40" s="47" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="32"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="32"/>
-      <c r="C26" s="36"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="D27" s="24" t="s">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="27"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="E27" s="37" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="32"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="24" t="s">
+      <c r="E41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D42" s="24" t="s">
         <v>148</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="K42" s="14" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Filtering works for entity sets
</commit_message>
<xml_diff>
--- a/MR3/Extensions/OData/tests/test odata stuff.xlsx
+++ b/MR3/Extensions/OData/tests/test odata stuff.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="164">
   <si>
     <t>Missing features</t>
   </si>
@@ -2462,8 +2462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,7 +2641,9 @@
       <c r="K10" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="L10" s="24"/>
+      <c r="L10" s="24" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
@@ -2879,7 +2881,9 @@
       <c r="K19" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="L19" s="24"/>
+      <c r="L19" s="24" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -2904,6 +2908,21 @@
       <c r="E21" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="F21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="K21" s="4" t="s">
         <v>135</v>
       </c>
@@ -2918,6 +2937,21 @@
       <c r="E22" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="F22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="K22" s="4" t="s">
         <v>135</v>
       </c>
@@ -2931,6 +2965,21 @@
       <c r="E23" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="F23" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="K23" s="4" t="s">
         <v>135</v>
       </c>
@@ -2953,6 +3002,21 @@
       </c>
       <c r="E26" s="4" t="s">
         <v>135</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>135</v>
@@ -2967,6 +3031,21 @@
       <c r="E27" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="F27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="K27" s="4" t="s">
         <v>135</v>
       </c>
@@ -2994,6 +3073,18 @@
       <c r="F31" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="G31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="27"/>
@@ -3007,6 +3098,18 @@
       <c r="F32" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="G32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="27"/>
@@ -3020,6 +3123,18 @@
       <c r="F33" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="G33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D34" s="24" t="s">
@@ -3029,6 +3144,18 @@
         <v>135</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3055,7 +3182,16 @@
       <c r="F37" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="G37" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="H37" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3071,7 +3207,16 @@
       <c r="F38" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="G38" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="H38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added a few tests
</commit_message>
<xml_diff>
--- a/MR3/Extensions/OData/tests/test odata stuff.xlsx
+++ b/MR3/Extensions/OData/tests/test odata stuff.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="19200" windowHeight="9525" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="19200" windowHeight="9525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="missing" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="164">
   <si>
     <t>Missing features</t>
   </si>
@@ -853,44 +853,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="5" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="5" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1436,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,10 +1461,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="15"/>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="35"/>
+      <c r="H1" s="45"/>
       <c r="I1" s="18"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
@@ -1511,16 +1511,16 @@
       <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="H5" s="38" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="H5" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="47"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
@@ -1863,12 +1863,12 @@
     </row>
     <row r="23" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1911,12 +1911,12 @@
     </row>
     <row r="27" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1968,12 +1968,12 @@
     </row>
     <row r="31" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -2049,15 +2049,18 @@
     </row>
     <row r="37" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="F38" s="4" t="s">
         <v>19</v>
       </c>
@@ -2161,12 +2164,12 @@
     </row>
     <row r="45" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
-      <c r="C45" s="36" t="s">
+      <c r="C45" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -2209,12 +2212,12 @@
     </row>
     <row r="49" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
-      <c r="C49" s="36" t="s">
+      <c r="C49" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -2253,12 +2256,12 @@
     </row>
     <row r="53" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="36" t="s">
+      <c r="C53" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
       <c r="I53" s="13"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -2287,12 +2290,12 @@
     </row>
     <row r="57" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
-      <c r="C57" s="36" t="s">
+      <c r="C57" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -2308,12 +2311,12 @@
     </row>
     <row r="60" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="36" t="s">
+      <c r="C60" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -2352,12 +2355,12 @@
     </row>
     <row r="64" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="36" t="s">
+      <c r="C64" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="44"/>
       <c r="I64" s="13"/>
     </row>
     <row r="65" spans="9:11" x14ac:dyDescent="0.25">
@@ -2371,12 +2374,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C31:F31"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="C45:F45"/>
@@ -2384,6 +2381,12 @@
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2462,7 +2465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
@@ -2476,33 +2479,33 @@
     <col min="15" max="19" width="9.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" s="44" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+    <row r="2" spans="2:19" s="40" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="40"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="33"/>
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
-      <c r="G2" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="42" t="s">
+      <c r="G2" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -2616,7 +2619,7 @@
       <c r="C9" s="30"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="42" t="s">
         <v>160</v>
       </c>
       <c r="C10" s="30"/>
@@ -2648,7 +2651,7 @@
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
       <c r="C11" s="30"/>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="41" t="s">
         <v>127</v>
       </c>
       <c r="E11" s="25" t="s">
@@ -2678,7 +2681,7 @@
       <c r="C12" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="41" t="s">
         <v>120</v>
       </c>
       <c r="E12" s="25" t="s">
@@ -2708,7 +2711,7 @@
       <c r="C13" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="41" t="s">
         <v>121</v>
       </c>
       <c r="E13" s="25" t="s">
@@ -2738,7 +2741,7 @@
       <c r="C14" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="41" t="s">
         <v>122</v>
       </c>
       <c r="E14" s="25" t="s">
@@ -2766,7 +2769,7 @@
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
       <c r="C15" s="30"/>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="41" t="s">
         <v>123</v>
       </c>
       <c r="E15" s="25" t="s">
@@ -2794,7 +2797,7 @@
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="27"/>
       <c r="C16" s="30"/>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="41" t="s">
         <v>128</v>
       </c>
       <c r="E16" s="25" t="s">
@@ -2822,7 +2825,7 @@
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="27"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="41" t="s">
         <v>130</v>
       </c>
       <c r="E17" s="25" t="s">
@@ -3057,7 +3060,7 @@
       <c r="C30" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="E30" s="47" t="s">
+      <c r="E30" s="43" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3166,7 +3169,7 @@
       <c r="C36" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="E36" s="47" t="s">
+      <c r="E36" s="43" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3231,7 +3234,7 @@
       <c r="C40" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="E40" s="47" t="s">
+      <c r="E40" s="43" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>